<commit_message>
Fix bug and update logic
</commit_message>
<xml_diff>
--- a/filled_recon.xlsx
+++ b/filled_recon.xlsx
@@ -334,7 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -402,14 +402,15 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,7 +840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:D34"/>
+  <dimension ref="A5:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="77" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -910,7 +911,7 @@
       <c r="B11" s="13" t="n"/>
       <c r="C11" s="14" t="n"/>
       <c r="D11" s="1" t="n">
-        <v>378837.27</v>
+        <v>109144.35</v>
       </c>
     </row>
     <row r="12">
@@ -941,7 +942,7 @@
       <c r="B14" s="37" t="n"/>
       <c r="C14" s="38" t="n"/>
       <c r="D14" s="39" t="n">
-        <v>211294.85</v>
+        <v>62822.81</v>
       </c>
     </row>
     <row r="15">
@@ -955,211 +956,103 @@
       <c r="D15" s="38" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="36" t="inlineStr">
-        <is>
-          <t>DXB/SI-62099</t>
-        </is>
-      </c>
+      <c r="A16" s="36" t="n"/>
       <c r="B16" s="36" t="n"/>
-      <c r="C16" s="38" t="n">
-        <v>2100</v>
-      </c>
+      <c r="C16" s="38" t="n"/>
       <c r="D16" s="38" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="36" t="inlineStr">
-        <is>
-          <t>DXB/SI-62100</t>
+      <c r="A17" s="40" t="inlineStr">
+        <is>
+          <t>Payment not booked</t>
         </is>
       </c>
       <c r="B17" s="36" t="n"/>
-      <c r="C17" s="38" t="n">
-        <v>44.1</v>
-      </c>
+      <c r="C17" s="38" t="n"/>
       <c r="D17" s="38" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="36" t="inlineStr">
         <is>
-          <t>AUH/SI-39045</t>
+          <t>Payment not recorded as per SOA (97591)</t>
         </is>
       </c>
       <c r="B18" s="36" t="n"/>
       <c r="C18" s="38" t="n">
-        <v>18375</v>
+        <v>1170.75</v>
       </c>
       <c r="D18" s="38" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="36" t="inlineStr">
         <is>
-          <t>DXB/SI-62533</t>
+          <t>Payment not recorded as per SOA (97625)</t>
         </is>
       </c>
       <c r="B19" s="36" t="n"/>
       <c r="C19" s="38" t="n">
-        <v>1323</v>
+        <v>8032.5</v>
       </c>
       <c r="D19" s="38" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="36" t="inlineStr">
-        <is>
-          <t>AUH/SI-39192</t>
-        </is>
-      </c>
-      <c r="B20" s="36" t="n"/>
-      <c r="C20" s="38" t="n">
-        <v>18375</v>
+      <c r="A20" s="41" t="inlineStr">
+        <is>
+          <t>Payment not recorded as per SOA (97758)</t>
+        </is>
+      </c>
+      <c r="B20" s="41" t="n"/>
+      <c r="C20" s="42" t="n">
+        <v>53619.56</v>
       </c>
       <c r="D20" s="38" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="36" t="inlineStr">
-        <is>
-          <t>AUH/SI-39207</t>
-        </is>
-      </c>
-      <c r="B21" s="36" t="n"/>
-      <c r="C21" s="36" t="n">
-        <v>9187.5</v>
-      </c>
-      <c r="D21" s="36" t="n"/>
+      <c r="A21" s="43" t="inlineStr">
+        <is>
+          <t>Vendor Claimed Total</t>
+        </is>
+      </c>
+      <c r="B21" s="44" t="n"/>
+      <c r="C21" s="44" t="n"/>
+      <c r="D21" s="45" t="n">
+        <v>171967.16</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="36" t="inlineStr">
-        <is>
-          <t>AUH/SI-39253</t>
-        </is>
-      </c>
-      <c r="B22" s="36" t="n"/>
-      <c r="C22" s="36" t="n">
-        <v>3543.75</v>
-      </c>
-      <c r="D22" s="36" t="n"/>
+      <c r="A22" s="44" t="n"/>
+      <c r="B22" s="44" t="n"/>
+      <c r="C22" s="44" t="n"/>
+      <c r="D22" s="46" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="36" t="inlineStr">
-        <is>
-          <t>AUH/SI-39360</t>
-        </is>
-      </c>
-      <c r="B23" s="36" t="n"/>
-      <c r="C23" s="36" t="n">
-        <v>117301.1</v>
-      </c>
-      <c r="D23" s="41" t="n"/>
+      <c r="A23" s="43" t="inlineStr">
+        <is>
+          <t>Adjusted Books Balance</t>
+        </is>
+      </c>
+      <c r="B23" s="44" t="n"/>
+      <c r="C23" s="44" t="n"/>
+      <c r="D23" s="47" t="n">
+        <v>171967.16</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="36" t="inlineStr">
-        <is>
-          <t>DXB/SI-62749</t>
-        </is>
-      </c>
-      <c r="B24" s="36" t="n"/>
-      <c r="C24" s="36" t="n">
-        <v>1323</v>
-      </c>
-      <c r="D24" s="36" t="n"/>
+      <c r="A24" s="44" t="n"/>
+      <c r="B24" s="44" t="n"/>
+      <c r="C24" s="44" t="n"/>
+      <c r="D24" s="46" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="36" t="inlineStr">
-        <is>
-          <t>DXB/SI-62797</t>
-        </is>
-      </c>
-      <c r="B25" s="36" t="n"/>
-      <c r="C25" s="36" t="n">
-        <v>8104.69</v>
-      </c>
-      <c r="D25" s="36" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="36" t="inlineStr">
-        <is>
-          <t>DXB/SI-63066</t>
-        </is>
-      </c>
-      <c r="B26" s="36" t="n"/>
-      <c r="C26" s="36" t="n">
-        <v>29385.27</v>
-      </c>
-      <c r="D26" s="36" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="36" t="n"/>
-      <c r="B27" s="36" t="n"/>
-      <c r="C27" s="36" t="n"/>
-      <c r="D27" s="36" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="40" t="inlineStr">
-        <is>
-          <t>Payment not booked</t>
-        </is>
-      </c>
-      <c r="B28" s="36" t="n"/>
-      <c r="C28" s="36" t="n"/>
-      <c r="D28" s="36" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="42" t="inlineStr">
-        <is>
-          <t>Payment not recorded as per SOA (DXB/SI-62494)</t>
-        </is>
-      </c>
-      <c r="B29" s="42" t="n"/>
-      <c r="C29" s="42" t="n">
-        <v>2232.44</v>
-      </c>
-      <c r="D29" s="36" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="43" t="inlineStr">
-        <is>
-          <t>Vendor Claimed Total</t>
-        </is>
-      </c>
-      <c r="B30" s="44" t="n"/>
-      <c r="C30" s="44" t="n"/>
-      <c r="D30" s="45" t="n">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="44" t="n"/>
-      <c r="B31" s="44" t="n"/>
-      <c r="C31" s="44" t="n"/>
-      <c r="D31" s="46" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="43" t="inlineStr">
-        <is>
-          <t>Adjusted Books Balance</t>
-        </is>
-      </c>
-      <c r="B32" s="44" t="n"/>
-      <c r="C32" s="44" t="n"/>
-      <c r="D32" s="45" t="n">
-        <v>590132.12</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="44" t="n"/>
-      <c r="B33" s="44" t="n"/>
-      <c r="C33" s="44" t="n"/>
-      <c r="D33" s="46" t="n"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="47" t="inlineStr">
+      <c r="A25" s="48" t="inlineStr">
         <is>
           <t>Difference</t>
         </is>
       </c>
-      <c r="B34" s="44" t="n"/>
-      <c r="C34" s="44" t="n"/>
-      <c r="D34" s="48" t="n">
-        <v>409867.88</v>
+      <c r="B25" s="44" t="n"/>
+      <c r="C25" s="44" t="n"/>
+      <c r="D25" s="49" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>